<commit_message>
Add New Sequence name: Friend_Request_Management Functions: Accept and reject the friend requests.
</commit_message>
<xml_diff>
--- a/Config_Folder/Config_File.xlsx
+++ b/Config_Folder/Config_File.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehwi\Documents\UiPath\Facebook Automation Complete POC\Config_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D273BC2-7372-4429-BA48-C2CF95601E34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30A36E1-36AF-4773-8B3A-99A378D170E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Friend_Request_Management" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -33,13 +34,22 @@
     <t>Password</t>
   </si>
   <si>
-    <t>email@gmail.com</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Always write the login details in 2nd Row</t>
+  </si>
+  <si>
+    <t>Cancel Friend Requests</t>
+  </si>
+  <si>
+    <t>Accept Friend Requests</t>
+  </si>
+  <si>
+    <t>Always write in the column no 2 of the sheet.</t>
+  </si>
+  <si>
+    <t>Skip FRM</t>
   </si>
 </sst>
 </file>
@@ -84,9 +94,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -371,12 +384,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -389,24 +402,62 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1234</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7508D07D-DF53-4CF1-8CF7-CFE69A2DE5CF}"/>
-  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7FA9A-C7E1-48E9-B2CA-BD4EDB3B24AA}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="71.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1) Updated the selector. 2) Added the Delay in the login button click activity.
</commit_message>
<xml_diff>
--- a/Config_Folder/Config_File.xlsx
+++ b/Config_Folder/Config_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehwi\Documents\UiPath\Facebook Automation Complete POC\Config_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30A36E1-36AF-4773-8B3A-99A378D170E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426EC1A-B9B3-4486-BEBD-571EC5220F09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Email</t>
   </si>
@@ -50,13 +50,19 @@
   </si>
   <si>
     <t>Skip FRM</t>
+  </si>
+  <si>
+    <t>rhassnain@gmail.com</t>
+  </si>
+  <si>
+    <t>Raza#123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +77,21 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Webdings"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Webdings"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,12 +115,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -383,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,14 +427,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E5ED75B9-2918-4757-A36A-A8AF08787B50}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -420,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7FA9A-C7E1-48E9-B2CA-BD4EDB3B24AA}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,14 +479,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="2"/>
+      <c r="D3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Logic that build:   - the number you enter in the sheer will cancel or accept the friend request accordingly.
</commit_message>
<xml_diff>
--- a/Config_Folder/Config_File.xlsx
+++ b/Config_Folder/Config_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehwi\Documents\UiPath\Facebook Automation Complete POC\Config_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426EC1A-B9B3-4486-BEBD-571EC5220F09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9782F04C-E9E7-4D8A-B444-7542B119B3BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,10 +479,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>50</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added a new sequence. (Unfriend_Facebook_Friends) Just enter the number in the sheet and the bot will unfriend the Facebook friends according to that number.
</commit_message>
<xml_diff>
--- a/Config_Folder/Config_File.xlsx
+++ b/Config_Folder/Config_File.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehwi\Documents\UiPath\Facebook Automation Complete POC\Config_Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9782F04C-E9E7-4D8A-B444-7542B119B3BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57080362-A6EC-448F-A9B8-A173AC2ECC7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Info" sheetId="1" r:id="rId1"/>
     <sheet name="Friend_Request_Management" sheetId="2" r:id="rId2"/>
+    <sheet name="Unfriend_Facebook_Friends" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Email</t>
   </si>
@@ -56,6 +57,15 @@
   </si>
   <si>
     <t>Raza#123</t>
+  </si>
+  <si>
+    <t>Skip FRM: when you write yes the seq. will execute otherwise it will skipped.</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No_Frineds_to_Remove</t>
   </si>
 </sst>
 </file>
@@ -451,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7FA9A-C7E1-48E9-B2CA-BD4EDB3B24AA}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,18 +488,45 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C6A461-D798-482A-9D87-62E303412079}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>